<commit_message>
Extend column filter for iteration Excel template
</commit_message>
<xml_diff>
--- a/SAP_Adapter/IterationResultsTemplate.xlsx
+++ b/SAP_Adapter/IterationResultsTemplate.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgreenro\Documents\Repo Code\BHoM\SAP_Toolkit\SAP_Adapter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rboulton\Desktop\Github\SAP_Toolkit\SAP_Adapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44F5ED7-C042-4D5B-AAE0-0D9F326B2680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2BAFFC-9AF7-4715-8EE0-DEBB78F8CB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA28078-BF63-4819-B9F5-45E4611DA917}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA28078-BF63-4819-B9F5-45E4611DA917}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$10:$K$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$10:$AD$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -383,56 +383,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -470,20 +421,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <bgColor theme="0"/>
         </patternFill>
@@ -493,132 +430,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -948,7 +759,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7E8FC2-D259-4B22-A7E5-4A5DEF497953}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1389,42 +1202,42 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A10:K10" xr:uid="{9B7E8FC2-D259-4B22-A7E5-4A5DEF497953}"/>
+  <autoFilter ref="A10:AD10" xr:uid="{9B7E8FC2-D259-4B22-A7E5-4A5DEF497953}"/>
   <mergeCells count="3">
     <mergeCell ref="Y6:Z6"/>
     <mergeCell ref="AA6:AB6"/>
     <mergeCell ref="AC6:AD6"/>
   </mergeCells>
   <conditionalFormatting sqref="R11:R1048576">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="greaterThanOrEqual">
       <formula>$B$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="lessThan">
       <formula>$B$3</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="15" priority="15">
+    <cfRule type="containsBlanks" dxfId="6" priority="15">
       <formula>LEN(TRIM(R11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11:U1048576">
-    <cfRule type="containsBlanks" dxfId="14" priority="6">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(U11))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="19" operator="greaterThanOrEqual">
       <formula>$C$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="lessThan">
       <formula>$C$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X11:X1048576">
-    <cfRule type="containsBlanks" dxfId="9" priority="4">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(X11))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="17" operator="greaterThanOrEqual">
       <formula>$D$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="lessThan">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>